<commit_message>
Started temperature data aggregation process
</commit_message>
<xml_diff>
--- a/USDA2020_prod_data/USDA2020_corn_prod.xlsx
+++ b/USDA2020_prod_data/USDA2020_corn_prod.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdavis\OneDrive - American Bankers Association\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdavis\OneDrive - American Bankers Association\Desktop\ag_futures\USDA2020_prod_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95BA499-1CC3-40FD-9ADF-64A73F57FA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CBDE31-003C-43A1-9B10-AB7643C8AA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="43200" yWindow="4065" windowWidth="18000" windowHeight="7605" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USDA2020_corn_prod" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="75">
   <si>
     <t>Program</t>
   </si>
@@ -276,6 +276,15 @@
   </si>
   <si>
     <t>Cumulative share of production</t>
+  </si>
+  <si>
+    <t>Last included state 1</t>
+  </si>
+  <si>
+    <t>Last included state 2</t>
+  </si>
+  <si>
+    <t>Last included state 3</t>
   </si>
 </sst>
 </file>
@@ -2790,10 +2799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F67C460-AAC4-4115-B87C-58963E074F9E}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2801,9 +2810,10 @@
     <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2814,7 +2824,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2827,7 +2837,7 @@
         <v>0.16180478702080842</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2840,7 +2850,7 @@
         <v>0.31204449663532074</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2853,7 +2863,7 @@
         <v>0.43819738143120529</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -2865,8 +2875,11 @@
         <f>SUM(B2:B5)</f>
         <v>0.53984604982805096</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2879,7 +2892,7 @@
         <v>0.60941721860030107</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -2892,7 +2905,7 @@
         <v>0.66373339832075362</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -2905,7 +2918,7 @@
         <v>0.71481957664305062</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -2917,8 +2930,11 @@
         <f>SUM(B2:B9)</f>
         <v>0.75480838289533558</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2931,7 +2947,7 @@
         <v>0.79455483274609151</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -2944,7 +2960,7 @@
         <v>0.83047531121715423</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2957,7 +2973,7 @@
         <v>0.85205140875327545</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2970,7 +2986,7 @@
         <v>0.86978452744292956</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2982,8 +2998,11 @@
         <f>SUM(B2:B14)</f>
         <v>0.88731780839798957</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -2996,7 +3015,7 @@
         <v>0.90373568299045703</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>62</v>
       </c>

</xml_diff>